<commit_message>
Add final components to PCB and added the missing footprints
</commit_message>
<xml_diff>
--- a/MotorBoard/BOM_MotorBoard .xlsx
+++ b/MotorBoard/BOM_MotorBoard .xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="252">
   <si>
     <t>Approved</t>
   </si>
@@ -571,9 +571,6 @@
     <t>1612060</t>
   </si>
   <si>
-    <t>2114873</t>
-  </si>
-  <si>
     <t>9731156</t>
   </si>
   <si>
@@ -758,6 +755,27 @@
   </si>
   <si>
     <t>Regulator fixed output 5V through hole</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/texas-instruments/LM317DCYR/296-12602-1-ND/443738</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/texas-instruments/UCC383T-5/296-8157-5-ND/373393</t>
+  </si>
+  <si>
+    <t>296-8157-5-ND</t>
+  </si>
+  <si>
+    <t>296-12602-1-ND</t>
+  </si>
+  <si>
+    <t>'Digi-Key</t>
+  </si>
+  <si>
+    <t>LM317DCYR</t>
+  </si>
+  <si>
+    <t>UCC383T-5</t>
   </si>
 </sst>
 </file>
@@ -768,7 +786,7 @@
     <numFmt numFmtId="164" formatCode="[$-C09]dd\-mmm\-yy;@"/>
     <numFmt numFmtId="165" formatCode="[$-409]h:mm:ss\ AM/PM;@"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -827,6 +845,18 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -1232,11 +1262,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="111">
+  <cellXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -1564,9 +1595,17 @@
     <xf numFmtId="0" fontId="10" fillId="5" borderId="18" xfId="1" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="15" xfId="2" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1874,8 +1913,8 @@
   </sheetPr>
   <dimension ref="A1:O76"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2045,11 +2084,11 @@
       </c>
       <c r="B8" s="9">
         <f ca="1">TODAY()</f>
-        <v>42821</v>
+        <v>42823</v>
       </c>
       <c r="C8" s="10">
         <f ca="1">NOW()</f>
-        <v>42821.649389351849</v>
+        <v>42823.499625578705</v>
       </c>
       <c r="D8" s="8"/>
       <c r="E8" s="3"/>
@@ -2166,25 +2205,25 @@
         <v>170</v>
       </c>
       <c r="I13" s="93" t="s">
+        <v>191</v>
+      </c>
+      <c r="J13" s="93" t="s">
         <v>192</v>
       </c>
-      <c r="J13" s="93" t="s">
-        <v>193</v>
-      </c>
       <c r="K13" s="93" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="L13" s="93" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="M13" s="93" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="N13" s="93" t="s">
+        <v>235</v>
+      </c>
+      <c r="O13" s="95" t="s">
         <v>236</v>
-      </c>
-      <c r="O13" s="95" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="14" spans="1:15" s="109" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2197,14 +2236,16 @@
         <v>74</v>
       </c>
       <c r="E14" s="104" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F14" s="105">
         <v>1</v>
       </c>
-      <c r="G14" s="106"/>
-      <c r="H14" s="106" t="s">
-        <v>128</v>
+      <c r="G14" s="106" t="s">
+        <v>249</v>
+      </c>
+      <c r="H14" s="112" t="s">
+        <v>247</v>
       </c>
       <c r="I14" s="106" t="s">
         <v>128</v>
@@ -2212,17 +2253,17 @@
       <c r="J14" s="106" t="s">
         <v>128</v>
       </c>
-      <c r="K14" s="106" t="s">
-        <v>212</v>
-      </c>
-      <c r="L14" s="106" t="s">
-        <v>128</v>
+      <c r="K14" s="111" t="s">
+        <v>246</v>
+      </c>
+      <c r="L14" s="113" t="s">
+        <v>251</v>
       </c>
       <c r="M14" s="106" t="s">
         <v>128</v>
       </c>
       <c r="N14" s="107" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="O14" s="108"/>
     </row>
@@ -2448,13 +2489,13 @@
         <v>169</v>
       </c>
       <c r="J20" s="94" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="K20" s="94" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L20" s="94" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="M20" s="94" t="s">
         <v>128</v>
@@ -2491,13 +2532,13 @@
         <v>168</v>
       </c>
       <c r="J21" s="94" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="K21" s="94" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="L21" s="94" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="M21" s="94" t="s">
         <v>128</v>
@@ -2537,10 +2578,10 @@
         <v>128</v>
       </c>
       <c r="K22" s="94" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="L22" s="94" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="M22" s="94" t="s">
         <v>128</v>
@@ -2578,10 +2619,10 @@
         <v>128</v>
       </c>
       <c r="K23" s="94" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="L23" s="94" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="M23" s="94" t="s">
         <v>128</v>
@@ -2619,10 +2660,10 @@
         <v>128</v>
       </c>
       <c r="K24" s="94" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="L24" s="94" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="M24" s="94" t="s">
         <v>128</v>
@@ -2660,13 +2701,13 @@
         <v>128</v>
       </c>
       <c r="K25" s="94" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L25" s="94" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="M25" s="94" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="N25" s="69">
         <v>47313</v>
@@ -2701,10 +2742,10 @@
         <v>128</v>
       </c>
       <c r="K26" s="94" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="L26" s="94" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="M26" s="94" t="s">
         <v>128</v>
@@ -2742,13 +2783,13 @@
         <v>128</v>
       </c>
       <c r="K27" s="94" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="L27" s="94" t="s">
         <v>128</v>
       </c>
       <c r="M27" s="94" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="N27" s="69"/>
       <c r="O27" s="80"/>
@@ -2781,10 +2822,10 @@
         <v>128</v>
       </c>
       <c r="K28" s="94" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="L28" s="94" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="M28" s="94" t="s">
         <v>128</v>
@@ -2822,10 +2863,10 @@
         <v>128</v>
       </c>
       <c r="K29" s="94" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="L29" s="94" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="M29" s="94" t="s">
         <v>128</v>
@@ -2863,13 +2904,13 @@
         <v>128</v>
       </c>
       <c r="K30" s="94" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="L30" s="94" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="M30" s="94" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="N30" s="69">
         <v>78637</v>
@@ -2886,16 +2927,16 @@
         <v>91</v>
       </c>
       <c r="E31" s="104" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F31" s="105">
         <v>1</v>
       </c>
       <c r="G31" s="106" t="s">
-        <v>128</v>
-      </c>
-      <c r="H31" s="106" t="s">
-        <v>128</v>
+        <v>169</v>
+      </c>
+      <c r="H31" s="113" t="s">
+        <v>248</v>
       </c>
       <c r="I31" s="106" t="s">
         <v>128</v>
@@ -2903,17 +2944,17 @@
       <c r="J31" s="106" t="s">
         <v>128</v>
       </c>
-      <c r="K31" s="106" t="s">
-        <v>212</v>
-      </c>
-      <c r="L31" s="106" t="s">
-        <v>128</v>
+      <c r="K31" s="111" t="s">
+        <v>245</v>
+      </c>
+      <c r="L31" s="113" t="s">
+        <v>250</v>
       </c>
       <c r="M31" s="106" t="s">
         <v>128</v>
       </c>
       <c r="N31" s="107" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="O31" s="108"/>
     </row>
@@ -2935,9 +2976,7 @@
       <c r="G32" s="94" t="s">
         <v>168</v>
       </c>
-      <c r="H32" s="94" t="s">
-        <v>183</v>
-      </c>
+      <c r="H32"/>
       <c r="I32" s="94" t="s">
         <v>128</v>
       </c>
@@ -2945,13 +2984,13 @@
         <v>128</v>
       </c>
       <c r="K32" s="94" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L32" s="94" t="s">
         <v>128</v>
       </c>
       <c r="M32" s="94" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="N32" s="69">
         <v>7073</v>
@@ -3445,7 +3484,7 @@
         <v>168</v>
       </c>
       <c r="H45" s="94" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I45" s="94" t="s">
         <v>128</v>
@@ -3454,13 +3493,13 @@
         <v>128</v>
       </c>
       <c r="K45" s="94" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="L45" s="94" t="s">
         <v>128</v>
       </c>
       <c r="M45" s="94" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="N45" s="69">
         <v>30986</v>
@@ -3486,7 +3525,7 @@
         <v>168</v>
       </c>
       <c r="H46" s="94" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="I46" s="94" t="s">
         <v>128</v>
@@ -3495,10 +3534,10 @@
         <v>128</v>
       </c>
       <c r="K46" s="94" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="L46" s="94" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="M46" s="94" t="s">
         <v>128</v>
@@ -3527,7 +3566,7 @@
         <v>168</v>
       </c>
       <c r="H47" s="94" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="I47" s="94" t="s">
         <v>128</v>
@@ -3536,10 +3575,10 @@
         <v>128</v>
       </c>
       <c r="K47" s="94" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="L47" s="94" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="M47" s="94" t="s">
         <v>128</v>
@@ -3568,7 +3607,7 @@
         <v>169</v>
       </c>
       <c r="H48" s="94" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I48" s="94" t="s">
         <v>128</v>
@@ -3577,10 +3616,10 @@
         <v>128</v>
       </c>
       <c r="K48" s="94" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="L48" s="94" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="M48" s="94" t="s">
         <v>128</v>
@@ -3609,7 +3648,7 @@
         <v>169</v>
       </c>
       <c r="H49" s="94" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="I49" s="94" t="s">
         <v>128</v>
@@ -3618,10 +3657,10 @@
         <v>128</v>
       </c>
       <c r="K49" s="94" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="L49" s="94" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="M49" s="94" t="s">
         <v>128</v>
@@ -3650,7 +3689,7 @@
         <v>169</v>
       </c>
       <c r="H50" s="94" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I50" s="94" t="s">
         <v>128</v>
@@ -3659,10 +3698,10 @@
         <v>128</v>
       </c>
       <c r="K50" s="94" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="L50" s="94" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="M50" s="94" t="s">
         <v>128</v>
@@ -3691,7 +3730,7 @@
         <v>169</v>
       </c>
       <c r="H51" s="94" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I51" s="94" t="s">
         <v>128</v>
@@ -3700,10 +3739,10 @@
         <v>128</v>
       </c>
       <c r="K51" s="94" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="L51" s="94" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="M51" s="94" t="s">
         <v>128</v>
@@ -3732,7 +3771,7 @@
         <v>169</v>
       </c>
       <c r="H52" s="94" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I52" s="94" t="s">
         <v>128</v>
@@ -3741,10 +3780,10 @@
         <v>128</v>
       </c>
       <c r="K52" s="94" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="L52" s="94" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="M52" s="94" t="s">
         <v>128</v>
@@ -3773,7 +3812,7 @@
         <v>169</v>
       </c>
       <c r="H53" s="94" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I53" s="94" t="s">
         <v>128</v>
@@ -3782,10 +3821,10 @@
         <v>128</v>
       </c>
       <c r="K53" s="94" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="L53" s="94" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="M53" s="94" t="s">
         <v>128</v>
@@ -3814,7 +3853,7 @@
         <v>169</v>
       </c>
       <c r="H54" s="94" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I54" s="94" t="s">
         <v>128</v>
@@ -3823,10 +3862,10 @@
         <v>128</v>
       </c>
       <c r="K54" s="94" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="L54" s="94" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="M54" s="94" t="s">
         <v>128</v>
@@ -3855,7 +3894,7 @@
         <v>169</v>
       </c>
       <c r="H55" s="94" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I55" s="94" t="s">
         <v>128</v>
@@ -3864,10 +3903,10 @@
         <v>128</v>
       </c>
       <c r="K55" s="94" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="L55" s="94" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="M55" s="94" t="s">
         <v>128</v>
@@ -3896,7 +3935,7 @@
         <v>169</v>
       </c>
       <c r="H56" s="94" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I56" s="94" t="s">
         <v>128</v>
@@ -3905,10 +3944,10 @@
         <v>128</v>
       </c>
       <c r="K56" s="94" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="L56" s="94" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="M56" s="94" t="s">
         <v>128</v>
@@ -3937,7 +3976,7 @@
         <v>169</v>
       </c>
       <c r="H57" s="94" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I57" s="94" t="s">
         <v>128</v>
@@ -3946,10 +3985,10 @@
         <v>128</v>
       </c>
       <c r="K57" s="94" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="L57" s="94" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="M57" s="94" t="s">
         <v>128</v>
@@ -3978,7 +4017,7 @@
         <v>169</v>
       </c>
       <c r="H58" s="94" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I58" s="94" t="s">
         <v>128</v>
@@ -3987,10 +4026,10 @@
         <v>128</v>
       </c>
       <c r="K58" s="94" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="L58" s="94" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="M58" s="94" t="s">
         <v>128</v>
@@ -4019,7 +4058,7 @@
         <v>169</v>
       </c>
       <c r="H59" s="94" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I59" s="94" t="s">
         <v>128</v>
@@ -4028,10 +4067,10 @@
         <v>128</v>
       </c>
       <c r="K59" s="94" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="L59" s="94" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="M59" s="94" t="s">
         <v>128</v>
@@ -4060,7 +4099,7 @@
         <v>169</v>
       </c>
       <c r="H60" s="94" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I60" s="94" t="s">
         <v>128</v>
@@ -4069,10 +4108,10 @@
         <v>128</v>
       </c>
       <c r="K60" s="94" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="L60" s="94" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="M60" s="94" t="s">
         <v>128</v>
@@ -4101,7 +4140,7 @@
         <v>169</v>
       </c>
       <c r="H61" s="94" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I61" s="94" t="s">
         <v>128</v>
@@ -4110,10 +4149,10 @@
         <v>128</v>
       </c>
       <c r="K61" s="94" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="L61" s="94" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="M61" s="94" t="s">
         <v>128</v>
@@ -4142,7 +4181,7 @@
         <v>169</v>
       </c>
       <c r="H62" s="94" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I62" s="94" t="s">
         <v>128</v>
@@ -4151,10 +4190,10 @@
         <v>128</v>
       </c>
       <c r="K62" s="94" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="L62" s="94" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="M62" s="94" t="s">
         <v>128</v>
@@ -4183,16 +4222,16 @@
         <v>168</v>
       </c>
       <c r="H63" s="94" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I63" s="94" t="s">
         <v>169</v>
       </c>
       <c r="J63" s="94" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="K63" s="94" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="L63" s="94" t="s">
         <v>69</v>
@@ -4224,7 +4263,7 @@
         <v>169</v>
       </c>
       <c r="H64" s="94" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="I64" s="94" t="s">
         <v>128</v>
@@ -4233,10 +4272,10 @@
         <v>128</v>
       </c>
       <c r="K64" s="94" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="L64" s="94" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="M64" s="94" t="s">
         <v>128</v>
@@ -4265,7 +4304,7 @@
         <v>169</v>
       </c>
       <c r="H65" s="94" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="I65" s="94" t="s">
         <v>128</v>
@@ -4274,10 +4313,10 @@
         <v>128</v>
       </c>
       <c r="K65" s="94" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="L65" s="94" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="M65" s="94" t="s">
         <v>128</v>
@@ -4306,7 +4345,7 @@
         <v>169</v>
       </c>
       <c r="H66" s="94" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I66" s="94" t="s">
         <v>128</v>
@@ -4315,10 +4354,10 @@
         <v>128</v>
       </c>
       <c r="K66" s="94" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="L66" s="94" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="M66" s="94" t="s">
         <v>128</v>
@@ -4507,8 +4546,12 @@
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="K31" r:id="rId1"/>
+    <hyperlink ref="K14" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.46" right="0.36" top="0.57999999999999996" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="200" verticalDpi="200" r:id="rId3"/>
   <headerFooter alignWithMargins="0">
     <oddFooter>&amp;L&amp;BAltium Limited Confidential&amp;B&amp;C&amp;D&amp;RPage &amp;P</oddFooter>
   </headerFooter>
@@ -4534,7 +4577,7 @@
         <v>7</v>
       </c>
       <c r="B1" s="96" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -4566,7 +4609,7 @@
         <v>11</v>
       </c>
       <c r="B5" s="98" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="6" spans="1:2" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -4582,7 +4625,7 @@
         <v>12</v>
       </c>
       <c r="B7" s="98" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="8" spans="1:2" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -4606,7 +4649,7 @@
         <v>16</v>
       </c>
       <c r="B10" s="97" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="11" spans="1:2" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -4622,7 +4665,7 @@
         <v>17</v>
       </c>
       <c r="B12" s="97" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="13" spans="1:2" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -4630,7 +4673,7 @@
         <v>18</v>
       </c>
       <c r="B13" s="98" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="14" spans="1:2" s="16" customFormat="1" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">

</xml_diff>